<commit_message>
excel upd 5 and DB script no data added
</commit_message>
<xml_diff>
--- a/BD_Shop.xlsx
+++ b/BD_Shop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="258">
   <si>
     <t>Роль сотрудника</t>
   </si>
@@ -636,9 +636,6 @@
     <t>Discount</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -648,9 +645,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>149</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -660,15 +654,9 @@
     <t>7</t>
   </si>
   <si>
-    <t>1200</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>86</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -678,94 +666,31 @@
     <t>17</t>
   </si>
   <si>
-    <t>166</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
-    <t>1700</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>4100</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <t>385</t>
-  </si>
-  <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
-    <t>510</t>
-  </si>
-  <si>
-    <t>2190</t>
-  </si>
-  <si>
-    <t>177</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
-    <t>640</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>3500</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>292</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>140</t>
-  </si>
-  <si>
     <t>20</t>
-  </si>
-  <si>
-    <t>50</t>
   </si>
   <si>
     <t>Picture</t>
@@ -974,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1006,6 +931,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1290,7 +1218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -1308,13 +1236,13 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1334,13 +1262,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -1360,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>31</v>
@@ -1386,13 +1314,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -1412,13 +1340,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>10</v>
@@ -1438,13 +1366,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -1464,13 +1392,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -1490,13 +1418,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
@@ -1516,13 +1444,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>21</v>
@@ -1542,13 +1470,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>24</v>
@@ -1568,13 +1496,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>27</v>
@@ -1742,9 +1670,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -2885,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2916,7 +2844,7 @@
         <v>103</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>104</v>
@@ -2931,19 +2859,19 @@
         <v>200</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>107</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>108</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>109</v>
@@ -2961,7 +2889,7 @@
         <v>112</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="94.5">
@@ -2981,11 +2909,11 @@
       <c r="E2" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="13">
+        <v>123</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="H2" s="5">
         <f>LOOKUP(I2,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3009,10 +2937,10 @@
         <v>117</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>118</v>
@@ -3041,11 +2969,11 @@
       <c r="E3" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>206</v>
+      <c r="F3" s="13">
+        <v>149</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H3" s="5">
         <f>LOOKUP(I3,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3069,10 +2997,10 @@
         <v>124</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>125</v>
@@ -3101,11 +3029,11 @@
       <c r="E4" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>210</v>
+      <c r="F4" s="13">
+        <v>1200</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H4" s="5">
         <f>LOOKUP(I4,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3129,10 +3057,10 @@
         <v>117</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>129</v>
@@ -3161,11 +3089,11 @@
       <c r="E5" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>212</v>
+      <c r="F5" s="13">
+        <v>86</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H5" s="5">
         <f>LOOKUP(I5,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3189,10 +3117,10 @@
         <v>133</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>134</v>
@@ -3221,11 +3149,11 @@
       <c r="E6" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>216</v>
+      <c r="F6" s="13">
+        <v>166</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H6" s="5">
         <f>LOOKUP(I6,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3249,10 +3177,10 @@
         <v>133</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>136</v>
@@ -3281,11 +3209,11 @@
       <c r="E7" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>218</v>
+      <c r="F7" s="13">
+        <v>1700</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H7" s="5">
         <f>LOOKUP(I7,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3309,10 +3237,10 @@
         <v>133</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>140</v>
@@ -3341,11 +3269,11 @@
       <c r="E8" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>220</v>
+      <c r="F8" s="13">
+        <v>300</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H8" s="5">
         <f>LOOKUP(I8,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3369,10 +3297,10 @@
         <v>133</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>144</v>
@@ -3401,11 +3329,11 @@
       <c r="E9" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>222</v>
+      <c r="F9" s="13">
+        <v>199</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H9" s="5">
         <f>LOOKUP(I9,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3429,10 +3357,10 @@
         <v>117</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>149</v>
@@ -3461,11 +3389,11 @@
       <c r="E10" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>223</v>
+      <c r="F10" s="13">
+        <v>234</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H10" s="5">
         <f>LOOKUP(I10,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3489,10 +3417,10 @@
         <v>133</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>153</v>
@@ -3521,11 +3449,11 @@
       <c r="E11" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>224</v>
+      <c r="F11" s="13">
+        <v>170</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H11" s="5">
         <f>LOOKUP(I11,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3549,10 +3477,10 @@
         <v>133</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>157</v>
@@ -3564,7 +3492,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="94.5">
+    <row r="12" spans="1:18" ht="78.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3581,11 +3509,11 @@
       <c r="E12" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>225</v>
+      <c r="F12" s="13">
+        <v>600</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H12" s="5">
         <f>LOOKUP(I12,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3609,10 +3537,10 @@
         <v>133</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>160</v>
@@ -3641,11 +3569,11 @@
       <c r="E13" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>220</v>
+      <c r="F13" s="13">
+        <v>300</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H13" s="5">
         <f>LOOKUP(I13,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3669,10 +3597,10 @@
         <v>133</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>161</v>
@@ -3701,11 +3629,11 @@
       <c r="E14" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>226</v>
+      <c r="F14" s="13">
+        <v>4100</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H14" s="5">
         <f>LOOKUP(I14,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3729,10 +3657,10 @@
         <v>117</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>164</v>
@@ -3761,11 +3689,11 @@
       <c r="E15" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>228</v>
+      <c r="F15" s="13">
+        <v>385</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H15" s="5">
         <f>LOOKUP(I15,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3789,10 +3717,10 @@
         <v>124</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>166</v>
@@ -3821,11 +3749,11 @@
       <c r="E16" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>229</v>
+      <c r="F16" s="13">
+        <v>280</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H16" s="5">
         <f>LOOKUP(I16,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3849,10 +3777,10 @@
         <v>117</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>168</v>
@@ -3881,11 +3809,11 @@
       <c r="E17" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>218</v>
+      <c r="F17" s="13">
+        <v>1700</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H17" s="5">
         <f>LOOKUP(I17,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3909,10 +3837,10 @@
         <v>133</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>170</v>
@@ -3941,11 +3869,11 @@
       <c r="E18" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>231</v>
+      <c r="F18" s="13">
+        <v>510</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H18" s="5">
         <f>LOOKUP(I18,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -3969,10 +3897,10 @@
         <v>133</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>171</v>
@@ -3984,7 +3912,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="94.5">
+    <row r="19" spans="1:18" ht="78.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4001,11 +3929,11 @@
       <c r="E19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>231</v>
+      <c r="F19" s="13">
+        <v>510</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H19" s="5">
         <f>LOOKUP(I19,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4029,10 +3957,10 @@
         <v>133</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>173</v>
@@ -4061,11 +3989,11 @@
       <c r="E20" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>232</v>
+      <c r="F20" s="13">
+        <v>2190</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H20" s="5">
         <f>LOOKUP(I20,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4089,10 +4017,10 @@
         <v>133</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>175</v>
@@ -4121,11 +4049,11 @@
       <c r="E21" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>233</v>
+      <c r="F21" s="13">
+        <v>177</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H21" s="5">
         <f>LOOKUP(I21,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4149,10 +4077,10 @@
         <v>133</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>177</v>
@@ -4181,11 +4109,11 @@
       <c r="E22" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>234</v>
+      <c r="F22" s="13">
+        <v>100</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H22" s="5">
         <f>LOOKUP(I22,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4209,10 +4137,10 @@
         <v>133</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>178</v>
@@ -4241,11 +4169,11 @@
       <c r="E23" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>236</v>
+      <c r="F23" s="13">
+        <v>640</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H23" s="5">
         <f>LOOKUP(I23,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4269,10 +4197,10 @@
         <v>133</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>179</v>
@@ -4301,11 +4229,11 @@
       <c r="E24" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>237</v>
+      <c r="F24" s="13">
+        <v>800</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H24" s="5">
         <f>LOOKUP(I24,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4329,10 +4257,10 @@
         <v>133</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>183</v>
@@ -4361,11 +4289,11 @@
       <c r="E25" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>238</v>
+      <c r="F25" s="13">
+        <v>3500</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H25" s="5">
         <f>LOOKUP(I25,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4389,10 +4317,10 @@
         <v>133</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P25" s="5" t="s">
         <v>186</v>
@@ -4421,11 +4349,11 @@
       <c r="E26" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>239</v>
+      <c r="F26" s="13">
+        <v>400</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H26" s="5">
         <f>LOOKUP(I26,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4449,10 +4377,10 @@
         <v>124</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>188</v>
@@ -4464,7 +4392,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="94.5">
+    <row r="27" spans="1:18" ht="78.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4481,11 +4409,11 @@
       <c r="E27" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>240</v>
+      <c r="F27" s="13">
+        <v>292</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="H27" s="5">
         <f>LOOKUP(I27,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4509,10 +4437,10 @@
         <v>124</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="P27" s="5" t="s">
         <v>190</v>
@@ -4541,11 +4469,11 @@
       <c r="E28" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>225</v>
+      <c r="F28" s="13">
+        <v>600</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H28" s="5">
         <f>LOOKUP(I28,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4569,10 +4497,10 @@
         <v>133</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>193</v>
@@ -4601,11 +4529,11 @@
       <c r="E29" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>243</v>
+      <c r="F29" s="13">
+        <v>140</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="H29" s="5">
         <f>LOOKUP(I29,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4629,10 +4557,10 @@
         <v>133</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>195</v>
@@ -4661,11 +4589,11 @@
       <c r="E30" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>245</v>
+      <c r="F30" s="13">
+        <v>50</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H30" s="5">
         <f>LOOKUP(I30,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4689,10 +4617,10 @@
         <v>133</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P30" s="5" t="s">
         <v>196</v>
@@ -4721,11 +4649,11 @@
       <c r="E31" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>225</v>
+      <c r="F31" s="13">
+        <v>600</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H31" s="5">
         <f>LOOKUP(I31,Manufacturer!$B$2:$B$14,Manufacturer!$A$2:$A$14)</f>
@@ -4749,10 +4677,10 @@
         <v>133</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>199</v>
@@ -4766,6 +4694,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>